<commit_message>
Database update logic implemented
</commit_message>
<xml_diff>
--- a/db/pharmacy/Read.xlsx
+++ b/db/pharmacy/Read.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BITS GOA\3rd Year\OOPS\Lab Assignments\Project\BPGC-Lifestyle\db\pharmacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4CD936-C72A-42C9-B9C6-EBF5840D1AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C70B713-84A5-44CC-9048-00BB3C21D627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -28,13 +28,29 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Crocin</t>
+    <t>crocin</t>
+  </si>
+  <si>
+    <t>Params</t>
+  </si>
+  <si>
+    <t>ex</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,28 +396,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D1" s="0"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>100</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>